<commit_message>
M3 outputs  -- CD A_R2 & CD B_R1
</commit_message>
<xml_diff>
--- a/Microbiome/MHeatmap_CD.xlsx
+++ b/Microbiome/MHeatmap_CD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyin/Dropbox (CSU Fullerton)/Research/Flies/Robert -- statistical analysis/Microbiome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF18D27-4C1A-8A43-ADB8-A686C257BA75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F421D304-6986-7D4A-BD18-451EDCF05BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="0" windowWidth="21360" windowHeight="17960" activeTab="1" xr2:uid="{D5804D24-12AA-FB4D-8DFD-87EF28224067}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17400" windowHeight="17960" activeTab="1" xr2:uid="{D5804D24-12AA-FB4D-8DFD-87EF28224067}"/>
   </bookViews>
   <sheets>
     <sheet name="4_23_18" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="55">
   <si>
     <t>Kingdom</t>
   </si>
@@ -193,13 +193,19 @@
   </si>
   <si>
     <t>A R2</t>
+  </si>
+  <si>
+    <t>B R1</t>
+  </si>
+  <si>
+    <t>B R2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,13 +236,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -251,22 +269,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,7 +608,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,34 +692,34 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>0.90986999999999996</v>
       </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
         <v>2.0518900000000002</v>
       </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
         <v>2.6553100000000001</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>5.2357699999999996</v>
       </c>
     </row>
@@ -719,34 +742,34 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
         <v>0.13319</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>0.56525000000000003</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>9.06E-2</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>1.07663</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>7.2450000000000001E-2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>5.2229999999999999E-2</v>
       </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
         <v>1.0183899999999999</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>0.98577999999999999</v>
       </c>
     </row>
@@ -769,34 +792,34 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>13.50755</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>12.06588</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>10.89466</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>8.8727499999999999</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="4">
         <v>11.430680000000001</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>13.386670000000001</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>17.446539999999999</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>10.22634</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <v>10.9964</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <v>14.58357</v>
       </c>
     </row>
@@ -819,34 +842,34 @@
       <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
         <v>0.25503999999999999</v>
       </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="5">
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
         <v>1.1150199999999999</v>
       </c>
     </row>
@@ -869,34 +892,34 @@
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>84.972849999999994</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>86.182919999999996</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>86.248329999999996</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>83.024850000000001</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>85.84178</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>82.808250000000001</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>76.68271</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>88.959190000000007</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <v>84.553979999999996</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="4">
         <v>77.705860000000001</v>
       </c>
     </row>
@@ -919,34 +942,34 @@
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>3.4009999999999999E-2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>0.31097000000000002</v>
       </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
         <v>4.0039999999999999E-2</v>
       </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
         <v>0.22631999999999999</v>
       </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
         <v>0.4834</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="4">
         <v>9.9019999999999997E-2</v>
       </c>
     </row>
@@ -969,34 +992,34 @@
       <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
         <v>1.5015700000000001</v>
       </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5">
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1019,34 +1042,34 @@
       <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>0.57571000000000006</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>1.3070299999999999</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>2.29176</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>4.4182899999999998</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <v>1.3958699999999999</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <v>3.5063200000000001</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>1.85442</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="4">
         <v>0.81445999999999996</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="4">
         <v>0.29250999999999999</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="4">
         <v>0.27496999999999999</v>
       </c>
     </row>
@@ -1069,34 +1092,34 @@
       <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
         <v>3.9641000000000002</v>
       </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1164,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B5163C-33F2-564A-BFD4-0E5AD3B6D2AC}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,10 +1205,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24" x14ac:dyDescent="0.2">
-      <c r="C1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1256,18 +1281,18 @@
       <c r="F3" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6">
         <v>0.28009000000000001</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1288,34 +1313,34 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="6">
         <v>49.109270000000002</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="6">
         <v>49.002040000000001</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="6">
         <v>14.515750000000001</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="6">
         <v>13.779059999999999</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="6">
         <v>23.145099999999999</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="6">
         <v>26.385459999999998</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="6">
         <v>23.792390000000001</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="6">
         <v>5.0438700000000001</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="6">
         <v>15.22926</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="6">
         <v>49.62941</v>
       </c>
     </row>
@@ -1338,34 +1363,34 @@
       <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="6">
         <v>49.354750000000003</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="6">
         <v>46.079160000000002</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="6">
         <v>84.425229999999999</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="6">
         <v>81.513149999999996</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="6">
         <v>76.020349999999993</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="6">
         <v>71.710800000000006</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="6">
         <v>76.207610000000003</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="6">
         <v>94.956130000000002</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="6">
         <v>84.770740000000004</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="6">
         <v>50.37059</v>
       </c>
     </row>
@@ -1388,22 +1413,22 @@
       <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="6">
         <v>1.5359799999999999</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="6">
         <v>4.9188000000000001</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="6">
         <v>1.0590200000000001</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1424,25 +1449,25 @@
       <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6">
         <v>4.7077900000000001</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="6">
         <v>0.55445999999999995</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="6">
         <v>1.90374</v>
       </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G8" s="3">
@@ -1487,11 +1512,13 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="24" x14ac:dyDescent="0.2">
-      <c r="C11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1562,16 +1589,16 @@
       <c r="F13" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1592,26 +1619,36 @@
       <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="6">
         <v>49.002040000000001</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="6">
         <v>15.06944</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="6">
         <v>19.623169999999998</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="6">
         <v>14.37157</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="6">
         <v>18.68601</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+      <c r="L14" s="6">
+        <v>24.03116</v>
+      </c>
+      <c r="M14" s="6">
+        <v>23.5883</v>
+      </c>
+      <c r="N14" s="6">
+        <v>18.603100000000001</v>
+      </c>
+      <c r="O14" s="6">
+        <v>17.667999999999999</v>
+      </c>
+      <c r="P14" s="6">
+        <v>43.038930000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1632,26 +1669,36 @@
       <c r="F15" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="6">
         <v>46.079160000000002</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="6">
         <v>83.032989999999998</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="6">
         <v>76.429429999999996</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="6">
         <v>81.044709999999995</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="6">
         <v>80.713120000000004</v>
       </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="L15" s="6">
+        <v>73.460549999999998</v>
+      </c>
+      <c r="M15" s="6">
+        <v>76.411699999999996</v>
+      </c>
+      <c r="N15" s="6">
+        <v>81.396900000000002</v>
+      </c>
+      <c r="O15" s="6">
+        <v>82.331999999999994</v>
+      </c>
+      <c r="P15" s="6">
+        <v>56.961069999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1672,21 +1719,22 @@
       <c r="F16" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="6">
         <v>4.9188000000000001</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="6">
         <v>1.89757</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="6">
         <v>3.9474</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1707,23 +1755,25 @@
       <c r="F17" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
         <v>4.5837199999999996</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="6">
         <v>0.60087000000000002</v>
       </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="L17" s="6">
+        <v>2.5082900000000001</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G18" s="3">
@@ -1748,30 +1798,590 @@
       </c>
       <c r="L18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P18" s="3">
         <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6">
+        <v>0.71045000000000003</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="6">
+        <v>38.278149999999997</v>
+      </c>
+      <c r="H24" s="6">
+        <v>14.815580000000001</v>
+      </c>
+      <c r="I24" s="6">
+        <v>12.472619999999999</v>
+      </c>
+      <c r="J24" s="6">
+        <v>16.695489999999999</v>
+      </c>
+      <c r="K24" s="6">
+        <v>20.50638</v>
+      </c>
+      <c r="L24" s="6">
+        <v>20.112169999999999</v>
+      </c>
+      <c r="M24" s="6">
+        <v>34.563360000000003</v>
+      </c>
+      <c r="N24" s="6">
+        <v>14.765890000000001</v>
+      </c>
+      <c r="O24" s="6">
+        <v>15.674939999999999</v>
+      </c>
+      <c r="P24" s="6">
+        <v>43.710830000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="6">
+        <v>61.721850000000003</v>
+      </c>
+      <c r="H25" s="6">
+        <v>85.184420000000003</v>
+      </c>
+      <c r="I25" s="6">
+        <v>85.803430000000006</v>
+      </c>
+      <c r="J25" s="6">
+        <v>76.416550000000001</v>
+      </c>
+      <c r="K25" s="6">
+        <v>77.974969999999999</v>
+      </c>
+      <c r="L25" s="6">
+        <v>75.923000000000002</v>
+      </c>
+      <c r="M25" s="6">
+        <v>65.436639999999997</v>
+      </c>
+      <c r="N25" s="6">
+        <v>85.234110000000001</v>
+      </c>
+      <c r="O25" s="6">
+        <v>84.325059999999993</v>
+      </c>
+      <c r="P25" s="6">
+        <v>56.289169999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6">
+        <v>1.7239599999999999</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6">
+        <v>6.8879599999999996</v>
+      </c>
+      <c r="K27" s="6">
+        <v>0.80818999999999996</v>
+      </c>
+      <c r="L27" s="6">
+        <v>3.9648300000000001</v>
+      </c>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="3">
+        <f>SUM(G23:G27)</f>
+        <v>100</v>
+      </c>
+      <c r="H28" s="3">
+        <f>SUM(H23:H27)</f>
+        <v>100</v>
+      </c>
+      <c r="I28" s="3">
+        <f>SUM(I23:I27)</f>
+        <v>100.00001</v>
+      </c>
+      <c r="J28" s="3">
+        <f>SUM(J23:J27)</f>
+        <v>100</v>
+      </c>
+      <c r="K28" s="3">
+        <f>SUM(K23:K27)</f>
+        <v>99.999989999999997</v>
+      </c>
+      <c r="L28" s="3">
+        <f>SUM(L23:L27)</f>
+        <v>100</v>
+      </c>
+      <c r="M28" s="3">
+        <f>SUM(M23:M27)</f>
+        <v>100</v>
+      </c>
+      <c r="N28" s="3">
+        <f>SUM(N23:N27)</f>
+        <v>100</v>
+      </c>
+      <c r="O28" s="3">
+        <f>SUM(O23:O27)</f>
+        <v>100</v>
+      </c>
+      <c r="P28" s="3">
+        <f>SUM(P23:P27)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="24" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" ref="G38:I38" si="2">SUM(G33:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <f>SUM(J33:J37)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" ref="K38:P38" si="3">SUM(K33:K37)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C11:D11"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A31:D31"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>